<commit_message>
uploaded a new version of transformer
</commit_message>
<xml_diff>
--- a/advanced/Transformer.xlsx
+++ b/advanced/Transformer.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://o365coloradoedu-my.sharepoint.com/personal/peye9704_colorado_edu/Documents/2024/AIbyHand/spreadsheets/github/ai-by-hand-excel/advanced/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tom/Library/CloudStorage/OneDrive-UCB-O365/2024/AIbyHand/spreadsheets/github/ai-by-hand-excel/advanced/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="470" documentId="8_{2E5A64D4-B270-824D-8CBE-5E6901D89F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB7DFA6B-5338-4E4D-B04A-7B1938609DA8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{935CCD55-BE3F-C842-8329-EF4DFD44467A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="740" windowWidth="24960" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,13 +42,7 @@
     <author>tc={70923F54-3559-094F-BE16-1664E7E198F6}</author>
     <author>tc={B98D24C8-17EF-9543-ABC8-2E47B523FADC}</author>
     <author>tc={85B1847A-EAFE-D34C-8936-324CB32A8C69}</author>
-    <author>tc={AA066A56-BF0B-F849-BBFF-96990A89DB97}</author>
-    <author>tc={575F9D59-2E1D-4149-827B-FAE2EC396ABC}</author>
     <author>tc={429757FA-6499-364E-B686-18036D7CE6FE}</author>
-    <author>tc={59D33A8F-C3A4-9D43-9107-14E53F1932A9}</author>
-    <author>tc={A0D0D70F-412C-D24A-B88A-012888FB50CA}</author>
-    <author>tc={5AD61CD2-8013-1648-843A-496DE8D97AF1}</author>
-    <author>tc={C294AE2C-7260-A246-9D1A-71AC1A72DEC8}</author>
     <author>tc={0D5BA982-E38C-B641-9D2B-43BA3FB8E7CC}</author>
     <author>tc={3389D202-7469-3447-B71D-7039948E7C2B}</author>
     <author>tc={B92B3D14-4EF5-AA44-94B2-CD7FCB4CC25E}</author>
@@ -104,35 +98,7 @@
 ↳ Note that the FFN is essentially a multi layer perceptron.</t>
       </text>
     </comment>
-    <comment ref="K18" authorId="5" shapeId="0" xr:uid="{AA066A56-BF0B-F849-BBFF-96990A89DB97}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    # FFN: First Layer
-↳ Feed all 5 attention weighted features into the first layer.
-↳ Multiply these features with the weights and biases.
-↳ The effect is to combine features across feature dimensions (vertically).
-↳ The dimensionality of each feature is decreased from 4 to 3.
-↳ Note that each position is processed by the same weight matrix. This is what the term "position-wise" is referring to.
-↳ Note that the FFN is essentially a multi layer perceptron.</t>
-      </text>
-    </comment>
-    <comment ref="L18" authorId="6" shapeId="0" xr:uid="{575F9D59-2E1D-4149-827B-FAE2EC396ABC}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    # FFN: First Layer
-↳ Feed all 5 attention weighted features into the first layer.
-↳ Multiply these features with the weights and biases.
-↳ The effect is to combine features across feature dimensions (vertically).
-↳ The dimensionality of each feature is decreased from 4 to 3.
-↳ Note that each position is processed by the same weight matrix. This is what the term "position-wise" is referring to.
-↳ Note that the FFN is essentially a multi layer perceptron.</t>
-      </text>
-    </comment>
-    <comment ref="P18" authorId="7" shapeId="0" xr:uid="{429757FA-6499-364E-B686-18036D7CE6FE}">
+    <comment ref="P18" authorId="5" shapeId="0" xr:uid="{429757FA-6499-364E-B686-18036D7CE6FE}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -141,63 +107,7 @@
 ↳ Negative values are set to zeros by ReLU.</t>
       </text>
     </comment>
-    <comment ref="J19" authorId="8" shapeId="0" xr:uid="{59D33A8F-C3A4-9D43-9107-14E53F1932A9}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    # FFN: First Layer
-↳ Feed all 5 attention weighted features into the first layer.
-↳ Multiply these features with the weights and biases.
-↳ The effect is to combine features across feature dimensions (vertically).
-↳ The dimensionality of each feature is decreased from 4 to 3.
-↳ Note that each position is processed by the same weight matrix. This is what the term "position-wise" is referring to.
-↳ Note that the FFN is essentially a multi layer perceptron.</t>
-      </text>
-    </comment>
-    <comment ref="K19" authorId="9" shapeId="0" xr:uid="{A0D0D70F-412C-D24A-B88A-012888FB50CA}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    # FFN: First Layer
-↳ Feed all 5 attention weighted features into the first layer.
-↳ Multiply these features with the weights and biases.
-↳ The effect is to combine features across feature dimensions (vertically).
-↳ The dimensionality of each feature is decreased from 4 to 3.
-↳ Note that each position is processed by the same weight matrix. This is what the term "position-wise" is referring to.
-↳ Note that the FFN is essentially a multi layer perceptron.</t>
-      </text>
-    </comment>
-    <comment ref="J20" authorId="10" shapeId="0" xr:uid="{5AD61CD2-8013-1648-843A-496DE8D97AF1}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    # FFN: First Layer
-↳ Feed all 5 attention weighted features into the first layer.
-↳ Multiply these features with the weights and biases.
-↳ The effect is to combine features across feature dimensions (vertically).
-↳ The dimensionality of each feature is decreased from 4 to 3.
-↳ Note that each position is processed by the same weight matrix. This is what the term "position-wise" is referring to.
-↳ Note that the FFN is essentially a multi layer perceptron.</t>
-      </text>
-    </comment>
-    <comment ref="K20" authorId="11" shapeId="0" xr:uid="{C294AE2C-7260-A246-9D1A-71AC1A72DEC8}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    # FFN: First Layer
-↳ Feed all 5 attention weighted features into the first layer.
-↳ Multiply these features with the weights and biases.
-↳ The effect is to combine features across feature dimensions (vertically).
-↳ The dimensionality of each feature is decreased from 4 to 3.
-↳ Note that each position is processed by the same weight matrix. This is what the term "position-wise" is referring to.
-↳ Note that the FFN is essentially a multi layer perceptron.</t>
-      </text>
-    </comment>
-    <comment ref="C23" authorId="12" shapeId="0" xr:uid="{0D5BA982-E38C-B641-9D2B-43BA3FB8E7CC}">
+    <comment ref="C23" authorId="6" shapeId="0" xr:uid="{0D5BA982-E38C-B641-9D2B-43BA3FB8E7CC}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -205,7 +115,7 @@
     The FFN layer combines features across dimensions (vertically).</t>
       </text>
     </comment>
-    <comment ref="P23" authorId="13" shapeId="0" xr:uid="{3389D202-7469-3447-B71D-7039948E7C2B}">
+    <comment ref="P23" authorId="7" shapeId="0" xr:uid="{3389D202-7469-3447-B71D-7039948E7C2B}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -217,7 +127,7 @@
 ↳ Note that the next block would have a completely separate set of parameters.</t>
       </text>
     </comment>
-    <comment ref="V23" authorId="14" shapeId="0" xr:uid="{B92B3D14-4EF5-AA44-94B2-CD7FCB4CC25E}">
+    <comment ref="V23" authorId="8" shapeId="0" xr:uid="{B92B3D14-4EF5-AA44-94B2-CD7FCB4CC25E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -228,6 +138,28 @@
     </comment>
   </commentList>
 </comments>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -363,7 +295,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -450,12 +382,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -878,7 +804,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -965,7 +891,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="1" applyFont="1" applyAlignment="1">
@@ -1480,63 +1406,9 @@
 ↳ Note that each position is processed by the same weight matrix. This is what the term "position-wise" is referring to.
 ↳ Note that the FFN is essentially a multi layer perceptron.</text>
   </threadedComment>
-  <threadedComment ref="K18" dT="2024-09-22T12:03:26.28" personId="{AEB4D18C-55B7-3040-AFB5-61A9D2B4C606}" id="{AA066A56-BF0B-F849-BBFF-96990A89DB97}">
-    <text># FFN: First Layer
-↳ Feed all 5 attention weighted features into the first layer.
-↳ Multiply these features with the weights and biases.
-↳ The effect is to combine features across feature dimensions (vertically).
-↳ The dimensionality of each feature is decreased from 4 to 3.
-↳ Note that each position is processed by the same weight matrix. This is what the term "position-wise" is referring to.
-↳ Note that the FFN is essentially a multi layer perceptron.</text>
-  </threadedComment>
-  <threadedComment ref="L18" dT="2024-09-22T12:03:26.28" personId="{AEB4D18C-55B7-3040-AFB5-61A9D2B4C606}" id="{575F9D59-2E1D-4149-827B-FAE2EC396ABC}">
-    <text># FFN: First Layer
-↳ Feed all 5 attention weighted features into the first layer.
-↳ Multiply these features with the weights and biases.
-↳ The effect is to combine features across feature dimensions (vertically).
-↳ The dimensionality of each feature is decreased from 4 to 3.
-↳ Note that each position is processed by the same weight matrix. This is what the term "position-wise" is referring to.
-↳ Note that the FFN is essentially a multi layer perceptron.</text>
-  </threadedComment>
   <threadedComment ref="P18" dT="2024-09-22T12:04:51.85" personId="{AEB4D18C-55B7-3040-AFB5-61A9D2B4C606}" id="{429757FA-6499-364E-B686-18036D7CE6FE}">
     <text># ReLU
 ↳ Negative values are set to zeros by ReLU.</text>
-  </threadedComment>
-  <threadedComment ref="J19" dT="2024-09-22T12:03:26.28" personId="{AEB4D18C-55B7-3040-AFB5-61A9D2B4C606}" id="{59D33A8F-C3A4-9D43-9107-14E53F1932A9}">
-    <text># FFN: First Layer
-↳ Feed all 5 attention weighted features into the first layer.
-↳ Multiply these features with the weights and biases.
-↳ The effect is to combine features across feature dimensions (vertically).
-↳ The dimensionality of each feature is decreased from 4 to 3.
-↳ Note that each position is processed by the same weight matrix. This is what the term "position-wise" is referring to.
-↳ Note that the FFN is essentially a multi layer perceptron.</text>
-  </threadedComment>
-  <threadedComment ref="K19" dT="2024-09-22T12:03:26.28" personId="{AEB4D18C-55B7-3040-AFB5-61A9D2B4C606}" id="{A0D0D70F-412C-D24A-B88A-012888FB50CA}">
-    <text># FFN: First Layer
-↳ Feed all 5 attention weighted features into the first layer.
-↳ Multiply these features with the weights and biases.
-↳ The effect is to combine features across feature dimensions (vertically).
-↳ The dimensionality of each feature is decreased from 4 to 3.
-↳ Note that each position is processed by the same weight matrix. This is what the term "position-wise" is referring to.
-↳ Note that the FFN is essentially a multi layer perceptron.</text>
-  </threadedComment>
-  <threadedComment ref="J20" dT="2024-09-22T12:03:26.28" personId="{AEB4D18C-55B7-3040-AFB5-61A9D2B4C606}" id="{5AD61CD2-8013-1648-843A-496DE8D97AF1}">
-    <text># FFN: First Layer
-↳ Feed all 5 attention weighted features into the first layer.
-↳ Multiply these features with the weights and biases.
-↳ The effect is to combine features across feature dimensions (vertically).
-↳ The dimensionality of each feature is decreased from 4 to 3.
-↳ Note that each position is processed by the same weight matrix. This is what the term "position-wise" is referring to.
-↳ Note that the FFN is essentially a multi layer perceptron.</text>
-  </threadedComment>
-  <threadedComment ref="K20" dT="2024-09-22T12:03:26.28" personId="{AEB4D18C-55B7-3040-AFB5-61A9D2B4C606}" id="{C294AE2C-7260-A246-9D1A-71AC1A72DEC8}">
-    <text># FFN: First Layer
-↳ Feed all 5 attention weighted features into the first layer.
-↳ Multiply these features with the weights and biases.
-↳ The effect is to combine features across feature dimensions (vertically).
-↳ The dimensionality of each feature is decreased from 4 to 3.
-↳ Note that each position is processed by the same weight matrix. This is what the term "position-wise" is referring to.
-↳ Note that the FFN is essentially a multi layer perceptron.</text>
   </threadedComment>
   <threadedComment ref="C23" dT="2024-09-22T23:51:43.78" personId="{AEB4D18C-55B7-3040-AFB5-61A9D2B4C606}" id="{0D5BA982-E38C-B641-9D2B-43BA3FB8E7CC}">
     <text>The FFN layer combines features across dimensions (vertically).</text>
@@ -1563,7 +1435,7 @@
   <dimension ref="A1:AB1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2301,21 +2173,21 @@
         <f t="array" ref="J18">MMULT($C18:$G18,J$12:J$16)</f>
         <v>7</v>
       </c>
-      <c r="K18" s="34">
+      <c r="K18" s="34" cm="1">
         <f t="array" ref="K18">MMULT($C18:$G18,K$12:K$16)</f>
         <v>13</v>
       </c>
-      <c r="L18" s="34">
+      <c r="L18" s="34" cm="1">
         <f t="array" ref="L18">MMULT($C18:$G18,L$12:L$16)</f>
         <v>11</v>
       </c>
-      <c r="M18" s="34">
-        <f t="array" ref="M18">MMULT($C18:$G18,M$6:M$10)</f>
-        <v>3</v>
-      </c>
-      <c r="N18" s="34">
-        <f t="array" ref="N18">MMULT($C18:$G18,N$6:N$10)</f>
-        <v>4</v>
+      <c r="M18" s="34" cm="1">
+        <f t="array" ref="M18">MMULT($C18:$G18,M$12:M$16)</f>
+        <v>9</v>
+      </c>
+      <c r="N18" s="34" cm="1">
+        <f t="array" ref="N18">MMULT($C18:$G18,N$12:N$16)</f>
+        <v>12</v>
       </c>
       <c r="O18" s="23" t="s">
         <v>16</v>
@@ -2334,11 +2206,11 @@
       </c>
       <c r="S18" s="34">
         <f t="shared" ref="S18:S20" si="2">IF(M18&gt;0, M18, 0)</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="T18" s="34">
         <f t="shared" ref="T18:T20" si="3">IF(N18&gt;0, N18, 0)</f>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="U18" s="1"/>
       <c r="V18" s="1"/>
@@ -2369,25 +2241,25 @@
         <v>3</v>
       </c>
       <c r="I19" s="46"/>
-      <c r="J19" s="34">
+      <c r="J19" s="34" cm="1">
         <f t="array" ref="J19">MMULT($C19:$G19,J$12:J$16)</f>
         <v>8</v>
       </c>
-      <c r="K19" s="34">
+      <c r="K19" s="34" cm="1">
         <f t="array" ref="K19">MMULT($C19:$G19,K$12:K$16)</f>
         <v>16</v>
       </c>
-      <c r="L19" s="34">
-        <f t="array" ref="L19">MMULT($C19:$G19,L$6:L$10)</f>
-        <v>6</v>
-      </c>
-      <c r="M19" s="34">
-        <f t="array" ref="M19">MMULT($C19:$G19,M$6:M$10)</f>
-        <v>2</v>
-      </c>
-      <c r="N19" s="34">
-        <f t="array" ref="N19">MMULT($C19:$G19,N$6:N$10)</f>
-        <v>5</v>
+      <c r="L19" s="34" cm="1">
+        <f t="array" ref="L19">MMULT($C19:$G19,L$12:L$16)</f>
+        <v>14</v>
+      </c>
+      <c r="M19" s="34" cm="1">
+        <f t="array" ref="M19">MMULT($C19:$G19,M$12:M$16)</f>
+        <v>10</v>
+      </c>
+      <c r="N19" s="34" cm="1">
+        <f t="array" ref="N19">MMULT($C19:$G19,N$12:N$16)</f>
+        <v>15</v>
       </c>
       <c r="O19" s="1" t="s">
         <v>17</v>
@@ -2402,15 +2274,15 @@
       </c>
       <c r="R19" s="34">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="S19" s="34">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="T19" s="34">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="U19" s="1"/>
       <c r="V19" s="1"/>
@@ -2441,25 +2313,25 @@
         <v>3</v>
       </c>
       <c r="I20" s="46"/>
-      <c r="J20" s="34">
+      <c r="J20" s="34" cm="1">
         <f t="array" ref="J20">MMULT($C20:$G20,J$12:J$16)</f>
         <v>1</v>
       </c>
-      <c r="K20" s="34">
+      <c r="K20" s="34" cm="1">
         <f t="array" ref="K20">MMULT($C20:$G20,K$12:K$16)</f>
         <v>5</v>
       </c>
-      <c r="L20" s="34">
-        <f t="array" ref="L20">MMULT($C20:$G20,L$6:L$10)</f>
-        <v>-1</v>
-      </c>
-      <c r="M20" s="34">
-        <f t="array" ref="M20">MMULT($C20:$G20,M$6:M$10)</f>
+      <c r="L20" s="34" cm="1">
+        <f t="array" ref="L20">MMULT($C20:$G20,L$12:L$16)</f>
+        <v>7</v>
+      </c>
+      <c r="M20" s="34" cm="1">
+        <f t="array" ref="M20">MMULT($C20:$G20,M$12:M$16)</f>
         <v>1</v>
       </c>
-      <c r="N20" s="34">
-        <f t="array" ref="N20">MMULT($C20:$G20,N$6:N$10)</f>
-        <v>0</v>
+      <c r="N20" s="34" cm="1">
+        <f t="array" ref="N20">MMULT($C20:$G20,N$12:N$16)</f>
+        <v>6</v>
       </c>
       <c r="O20" s="1" t="s">
         <v>17</v>
@@ -2474,7 +2346,7 @@
       </c>
       <c r="R20" s="34">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="S20" s="34">
         <f t="shared" si="2"/>
@@ -2482,7 +2354,7 @@
       </c>
       <c r="T20" s="34">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="U20" s="1"/>
       <c r="V20" s="1"/>
@@ -2607,15 +2479,15 @@
       </c>
       <c r="R23" s="34">
         <f t="array" ref="R23">MMULT($K23:$N23,R$18:R$21)</f>
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="S23" s="34">
         <f t="array" ref="S23">MMULT($K23:$N23,S$18:S$21)</f>
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="T23" s="34">
         <f t="array" ref="T23">MMULT($K23:$N23,T$18:T$21)</f>
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="U23" s="23" t="s">
         <v>16</v>
@@ -2630,15 +2502,15 @@
       </c>
       <c r="X23" s="34">
         <f t="shared" ref="X23:X26" si="6">IF(R23&gt;0, R23, 0)</f>
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="Y23" s="34">
         <f t="shared" ref="Y23:Y26" si="7">IF(S23&gt;0, S23, 0)</f>
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="Z23" s="34">
         <f t="shared" ref="Z23:Z26" si="8">IF(T23&gt;0, T23, 0)</f>
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="AA23" s="10"/>
     </row>
@@ -2681,11 +2553,11 @@
       </c>
       <c r="S24" s="34">
         <f t="array" ref="S24">MMULT($K24:$N24,S$18:S$21)</f>
-        <v>4</v>
+        <v>-2</v>
       </c>
       <c r="T24" s="34">
         <f t="array" ref="T24">MMULT($K24:$N24,T$18:T$21)</f>
-        <v>3</v>
+        <v>-5</v>
       </c>
       <c r="U24" s="1" t="s">
         <v>17</v>
@@ -2704,11 +2576,11 @@
       </c>
       <c r="Y24" s="34">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Z24" s="34">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AA24" s="10"/>
     </row>
@@ -2747,15 +2619,15 @@
       </c>
       <c r="R25" s="34">
         <f t="array" ref="R25">MMULT($K25:$N25,R$18:R$21)</f>
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="S25" s="34">
         <f t="array" ref="S25">MMULT($K25:$N25,S$18:S$21)</f>
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="T25" s="34">
         <f t="array" ref="T25">MMULT($K25:$N25,T$18:T$21)</f>
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="U25" s="1" t="s">
         <v>17</v>
@@ -2770,15 +2642,15 @@
       </c>
       <c r="X25" s="34">
         <f t="shared" si="6"/>
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="Y25" s="34">
         <f t="shared" si="7"/>
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="Z25" s="34">
         <f t="shared" si="8"/>
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="AA25" s="10"/>
     </row>
@@ -2817,7 +2689,7 @@
       </c>
       <c r="R26" s="34">
         <f t="array" ref="R26">MMULT($K26:$N26,R$18:R$21)</f>
-        <v>-1</v>
+        <v>-8</v>
       </c>
       <c r="S26" s="34">
         <f t="array" ref="S26">MMULT($K26:$N26,S$18:S$21)</f>
@@ -2825,7 +2697,7 @@
       </c>
       <c r="T26" s="34">
         <f t="array" ref="T26">MMULT($K26:$N26,T$18:T$21)</f>
-        <v>-1</v>
+        <v>-7</v>
       </c>
       <c r="U26" s="1" t="s">
         <v>17</v>
@@ -28244,7 +28116,7 @@
     <mergeCell ref="H19:I19"/>
     <mergeCell ref="H20:I20"/>
   </mergeCells>
-  <conditionalFormatting sqref="J12:N15 P18:T20 P23:T26 V23:Z26 J18:N20">
+  <conditionalFormatting sqref="J12:N15 J18:N20 P18:T20 P23:T26 V23:Z26">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>$U$2=TRUE</formula>
     </cfRule>
@@ -28262,7 +28134,7 @@
   <dimension ref="A1:AN1015"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -29567,7 +29439,7 @@
         <v>3</v>
       </c>
       <c r="L23" s="46"/>
-      <c r="M23" s="34">
+      <c r="M23" s="34" cm="1">
         <f t="array" ref="M23">MMULT($D23:$J23,M$15:M$21)</f>
         <v>4</v>
       </c>
@@ -68401,12 +68273,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A1:AN1"/>
-    <mergeCell ref="C2:J3"/>
-    <mergeCell ref="U6:AB7"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="U15:AB16"/>
-    <mergeCell ref="K16:L16"/>
     <mergeCell ref="A44:AN44"/>
     <mergeCell ref="K27:L27"/>
     <mergeCell ref="K28:L28"/>
@@ -68423,6 +68289,12 @@
     <mergeCell ref="K26:L26"/>
     <mergeCell ref="K29:L29"/>
     <mergeCell ref="K30:L30"/>
+    <mergeCell ref="A1:AN1"/>
+    <mergeCell ref="C2:J3"/>
+    <mergeCell ref="U6:AB7"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="U15:AB16"/>
+    <mergeCell ref="K16:L16"/>
   </mergeCells>
   <conditionalFormatting sqref="M15:T20 M23:T32 V23:AC32 V35:AC40 AE35:AL40">
     <cfRule type="expression" dxfId="0" priority="1">

</xml_diff>